<commit_message>
Drop ticket tipe "Problem" from Snowball
</commit_message>
<xml_diff>
--- a/ogv.xlsx
+++ b/ogv.xlsx
@@ -10,7 +10,9 @@
     <sheet name="tables" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Инциденты" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Консультации" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Старые обращения" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Старше 4 недель" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Старше 3 недель" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Старше 2 недель" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Отклонение_даты">#REF!</definedName>
@@ -276,12 +278,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$35:$RA$35</f>
+              <f>'tables'!$OM$35:$RE$35</f>
             </numRef>
           </val>
         </ser>
@@ -308,12 +310,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$36:$RA$36</f>
+              <f>'tables'!$OM$36:$RE$36</f>
             </numRef>
           </val>
         </ser>
@@ -340,12 +342,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$37:$RA$37</f>
+              <f>'tables'!$OM$37:$RE$37</f>
             </numRef>
           </val>
         </ser>
@@ -372,12 +374,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$38:$RA$38</f>
+              <f>'tables'!$OM$38:$RE$38</f>
             </numRef>
           </val>
         </ser>
@@ -404,12 +406,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$45:$RA$45</f>
+              <f>'tables'!$OM$45:$RE$45</f>
             </numRef>
           </val>
         </ser>
@@ -495,12 +497,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$86:$RA$86</f>
+              <f>'tables'!$OM$86:$RE$86</f>
             </numRef>
           </val>
         </ser>
@@ -527,12 +529,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$89:$RA$89</f>
+              <f>'tables'!$OM$89:$RE$89</f>
             </numRef>
           </val>
         </ser>
@@ -618,12 +620,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$54:$RA$54</f>
+              <f>'tables'!$OM$54:$RE$54</f>
             </numRef>
           </val>
         </ser>
@@ -650,12 +652,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$63:$RA$63</f>
+              <f>'tables'!$OM$63:$RE$63</f>
             </numRef>
           </val>
         </ser>
@@ -741,12 +743,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$68:$RA$68</f>
+              <f>'tables'!$OM$68:$RE$68</f>
             </numRef>
           </val>
         </ser>
@@ -832,12 +834,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$67:$RA$67</f>
+              <f>'tables'!$OM$67:$RE$67</f>
             </numRef>
           </val>
         </ser>
@@ -910,7 +912,7 @@
           </tx>
           <spPr>
             <a:solidFill>
-              <a:srgbClr val="98FB98"/>
+              <a:srgbClr val="C3D69B"/>
             </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -918,12 +920,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$75:$RA$75</f>
+              <f>'tables'!$OM$75:$RE$75</f>
             </numRef>
           </val>
         </ser>
@@ -937,7 +939,7 @@
           </tx>
           <spPr>
             <a:solidFill>
-              <a:srgbClr val="EEE8AA"/>
+              <a:srgbClr val="FFF2CC"/>
             </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -945,12 +947,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$76:$RA$76</f>
+              <f>'tables'!$OM$76:$RE$76</f>
             </numRef>
           </val>
         </ser>
@@ -964,7 +966,7 @@
           </tx>
           <spPr>
             <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -972,12 +974,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$77:$RA$77</f>
+              <f>'tables'!$OM$77:$RE$77</f>
             </numRef>
           </val>
         </ser>
@@ -991,7 +993,7 @@
           </tx>
           <spPr>
             <a:solidFill>
-              <a:srgbClr val="DC143C"/>
+              <a:srgbClr val="FF4F4F"/>
             </a:solidFill>
             <a:ln>
               <a:prstDash val="solid"/>
@@ -999,12 +1001,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$78:$RA$78</f>
+              <f>'tables'!$OM$78:$RE$78</f>
             </numRef>
           </val>
         </ser>
@@ -1084,12 +1086,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$81:$RA$81</f>
+              <f>'tables'!$OM$81:$RE$81</f>
             </numRef>
           </val>
         </ser>
@@ -1108,12 +1110,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$82:$RA$82</f>
+              <f>'tables'!$OM$82:$RE$82</f>
             </numRef>
           </val>
         </ser>
@@ -1193,12 +1195,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$72:$RA$72</f>
+              <f>'tables'!$OM$72:$RE$72</f>
             </numRef>
           </val>
         </ser>
@@ -1285,12 +1287,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$84:$RA$84</f>
+              <f>'tables'!$OM$84:$RE$84</f>
             </numRef>
           </val>
         </ser>
@@ -1317,12 +1319,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$85:$RA$85</f>
+              <f>'tables'!$OM$85:$RE$85</f>
             </numRef>
           </val>
         </ser>
@@ -1349,12 +1351,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$86:$RA$86</f>
+              <f>'tables'!$OM$86:$RE$86</f>
             </numRef>
           </val>
         </ser>
@@ -1381,12 +1383,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$87:$RA$87</f>
+              <f>'tables'!$OM$87:$RE$87</f>
             </numRef>
           </val>
         </ser>
@@ -1472,12 +1474,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'tables'!$OI$1:$RA$1</f>
+              <f>'tables'!$OM$1:$RE$1</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'tables'!$OI$88:$RA$88</f>
+              <f>'tables'!$OM$88:$RE$88</f>
             </numRef>
           </val>
         </ser>
@@ -1979,7 +1981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:RB89"/>
+  <dimension ref="A1:RF89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4328,17 +4330,37 @@
       </c>
       <c r="QZ1" s="4" t="inlineStr">
         <is>
-          <t>25.05.2023</t>
+          <t>26.05.2023</t>
         </is>
       </c>
       <c r="RA1" s="4" t="inlineStr">
         <is>
-          <t>26.05.2023</t>
+          <t>29.05.2023</t>
         </is>
       </c>
       <c r="RB1" s="4" t="inlineStr">
         <is>
-          <t>29.05.2023</t>
+          <t>30.05.2023</t>
+        </is>
+      </c>
+      <c r="RC1" s="4" t="inlineStr">
+        <is>
+          <t>1.06.2023</t>
+        </is>
+      </c>
+      <c r="RD1" s="4" t="inlineStr">
+        <is>
+          <t>2.06.2023</t>
+        </is>
+      </c>
+      <c r="RE1" s="4" t="inlineStr">
+        <is>
+          <t>29.06.2023</t>
+        </is>
+      </c>
+      <c r="RF1" s="4" t="inlineStr">
+        <is>
+          <t>30.06.2023</t>
         </is>
       </c>
     </row>
@@ -14868,8 +14890,14 @@
       <c r="QY37" t="n">
         <v>14</v>
       </c>
+      <c r="QZ37" t="n">
+        <v>13</v>
+      </c>
       <c r="RA37" t="n">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="RC37" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -14883,6 +14911,12 @@
           <t>Июнь 2023</t>
         </is>
       </c>
+      <c r="RC38" t="n">
+        <v>6</v>
+      </c>
+      <c r="RE38" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
@@ -15240,8 +15274,17 @@
       <c r="QY45" t="n">
         <v>14</v>
       </c>
+      <c r="QZ45" t="n">
+        <v>13</v>
+      </c>
       <c r="RA45" t="n">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="RC45" t="n">
+        <v>12</v>
+      </c>
+      <c r="RE45" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -22748,7 +22791,16 @@
       <c r="QY54" t="n">
         <v>0</v>
       </c>
+      <c r="QZ54" t="n">
+        <v>0</v>
+      </c>
       <c r="RA54" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC54" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -29667,7 +29719,16 @@
       <c r="QY63" t="n">
         <v>0</v>
       </c>
+      <c r="QZ63" t="n">
+        <v>0</v>
+      </c>
       <c r="RA63" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC63" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -31564,8 +31625,17 @@
       <c r="QY67" t="n">
         <v>2</v>
       </c>
+      <c r="QZ67" t="n">
+        <v>2</v>
+      </c>
       <c r="RA67" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="RC67" t="n">
+        <v>1</v>
+      </c>
+      <c r="RE67" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -32683,8 +32753,17 @@
       <c r="QY68" t="n">
         <v>76</v>
       </c>
+      <c r="QZ68" t="n">
+        <v>77</v>
+      </c>
       <c r="RA68" t="n">
-        <v>77</v>
+        <v>71</v>
+      </c>
+      <c r="RC68" t="n">
+        <v>60</v>
+      </c>
+      <c r="RE68" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="69">
@@ -36681,8 +36760,17 @@
       <c r="QY75" t="n">
         <v>12</v>
       </c>
+      <c r="QZ75" t="n">
+        <v>16</v>
+      </c>
       <c r="RA75" t="n">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="RC75" t="n">
+        <v>15</v>
+      </c>
+      <c r="RE75" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="76">
@@ -37140,8 +37228,17 @@
       <c r="QY76" t="n">
         <v>9</v>
       </c>
+      <c r="QZ76" t="n">
+        <v>10</v>
+      </c>
       <c r="RA76" t="n">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="RC76" t="n">
+        <v>8</v>
+      </c>
+      <c r="RE76" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -37594,13 +37691,22 @@
         <v>0</v>
       </c>
       <c r="QX77" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="QY77" t="n">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="QZ77" t="n">
+        <v>4</v>
       </c>
       <c r="RA77" t="n">
         <v>1</v>
+      </c>
+      <c r="RC77" t="n">
+        <v>2</v>
+      </c>
+      <c r="RE77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -38053,13 +38159,22 @@
         <v>0</v>
       </c>
       <c r="QX78" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="QY78" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="QZ78" t="n">
+        <v>4</v>
       </c>
       <c r="RA78" t="n">
         <v>0</v>
+      </c>
+      <c r="RC78" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE78" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -38415,7 +38530,16 @@
       <c r="QY81" t="n">
         <v>0</v>
       </c>
+      <c r="QZ81" t="n">
+        <v>0</v>
+      </c>
       <c r="RA81" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC81" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38788,8 +38912,17 @@
       <c r="QY84" t="n">
         <v>5</v>
       </c>
+      <c r="QZ84" t="n">
+        <v>5</v>
+      </c>
       <c r="RA84" t="n">
+        <v>4</v>
+      </c>
+      <c r="RC84" t="n">
         <v>5</v>
+      </c>
+      <c r="RE84" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -38858,7 +38991,16 @@
       <c r="QY85" t="n">
         <v>1</v>
       </c>
+      <c r="QZ85" t="n">
+        <v>0</v>
+      </c>
       <c r="RA85" t="n">
+        <v>1</v>
+      </c>
+      <c r="RC85" t="n">
+        <v>1</v>
+      </c>
+      <c r="RE85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -38928,8 +39070,17 @@
       <c r="QY86" t="n">
         <v>13</v>
       </c>
+      <c r="QZ86" t="n">
+        <v>6</v>
+      </c>
       <c r="RA86" t="n">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="RC86" t="n">
+        <v>4</v>
+      </c>
+      <c r="RE86" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="87">
@@ -38998,7 +39149,16 @@
       <c r="QY87" t="n">
         <v>0</v>
       </c>
+      <c r="QZ87" t="n">
+        <v>0</v>
+      </c>
       <c r="RA87" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC87" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -39069,12 +39229,24 @@
         <v>19</v>
       </c>
       <c r="QZ88" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="RA88" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="RB88" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC88" t="n">
+        <v>10</v>
+      </c>
+      <c r="RD88" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE88" t="n">
+        <v>9</v>
+      </c>
+      <c r="RF88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -39144,8 +39316,17 @@
       <c r="QY89" t="n">
         <v>4.65</v>
       </c>
+      <c r="QZ89" t="n">
+        <v>3</v>
+      </c>
       <c r="RA89" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="RC89" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="RE89" t="n">
+        <v>3.45</v>
       </c>
     </row>
   </sheetData>
@@ -39159,7 +39340,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39216,13 +39397,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595687</t>
+          <t xml:space="preserve">    597715</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Медленно выполняется первоначальная загрузка данных и каждое последующее обновление на клиенте Solo</t>
+          <t>Продолжение обращения №586817 "SSL connection could not be established", при запуске rxcmd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -39232,46 +39412,46 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>17.37</v>
+        <v>28.25</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Высокий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Интант ООО</t>
+          <t>РосА Ижевск</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595821</t>
+          <t xml:space="preserve">    598250</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>"Значение свойства Имя превышает допустимую длину строки (50)",  при работе ФП Получение сообщений из сервисов обмена</t>
+          <t>Продолжение обращения №596279 При выгрузке документов с открепленной ЭП расходится время подписания и установки штампа времени</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>В работе</t>
+          <t>На контроле</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>15.7</v>
+        <v>11.2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -39280,19 +39460,19 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>АрмаДок ООО</t>
+          <t>СТАРКОВ Групп ООО</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596047</t>
+          <t xml:space="preserve">    599475</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Некорректная установка службы Workflow</t>
+          <t>При заполнении карточек подразделений при попытке первого сохранения только что созданной карточки возникает ошибка "a different object with the same identifier value was already associated with the session: 89, of entity: Sungero.Company.Server.Departmen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -39302,11 +39482,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Банников Константин</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>12.9</v>
+        <v>10.68</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -39315,19 +39495,20 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Акелон ООО (Akelon)</t>
+          <t>Гарант-Чебоксары</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595701</t>
+          <t xml:space="preserve">    599378</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[RICUR#092676][EXT#2608] Внезапный запрос пароля в Directum Solo</t>
+          <t>В УПД поступающих в Директум из Диадок количество грузится не корректно. Округление до сотых, необходимо до тысячных как в Диадок. 
+Вопрос: как настроить Директум, чтобы округление было до тысячных</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -39337,11 +39518,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Банников Константин</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>11.63</v>
+        <v>10.62</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -39350,19 +39531,19 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Центр цифровых технологий УР (АУ ЦЦТ УР) (ПУР) (бывш. АУ РИЦ УР)</t>
+          <t>ЕАЕ-Консалт (EAE Consulting)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595715</t>
+          <t xml:space="preserve">    599065</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ошибка в работе сервисов Workflow "RabbitMQ channel #{channelNumber} (connection: '{connectionName}') shutdowned"</t>
+          <t>Не захватился пакет с электронной почты. В настройках приложений-обработчиков разрешение вложения *.jpeg прописано.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -39372,11 +39553,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>10.7</v>
+        <v>7.73</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -39385,19 +39566,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>АрмаДок ООО</t>
+          <t>Администрация Губернатора Владимирской области</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595636</t>
+          <t xml:space="preserve">    599595</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Exchange. Unknown counterparty with OrganizationId: 'da31050f-a71b-4193-86ce-d591715995b8'. It is necessary to synchronize counterparties. при получении сообщения из Диадок</t>
+          <t>[DTC#099444][EXT#2696] Классификатор (ИД=13) не найден после обновления на версии АРИО 2023.2.1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -39407,46 +39588,46 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Зверев Иван</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>10.43</v>
+        <v>6.28</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Средний</t>
+          <t>Низкий</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ГО Инвест (А-Инвестиции) ООО</t>
+          <t>Центр цифровых технологий УР (АУ ЦЦТ УР) (ПУР) (бывш. АУ РИЦ УР)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">    593913</t>
+          <t xml:space="preserve">    599613</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[RICUR#090153][EXT#2550] Ошибка при создании исходящего пакета с типом "Квитанция": не удалось создать папку при копировании пакета из папки. Функция MEDOCopyFiles: ошибка в строке 40</t>
+          <t>Не обрабатывается пакет МЭДО от конкретной организации</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Переадресовано</t>
+          <t>На контроле</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>9.9</v>
+        <v>6.03</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -39455,33 +39636,33 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Центр цифровых технологий УР (АУ ЦЦТ УР) (ПУР) (бывш. АУ РИЦ УР)</t>
+          <t>Агентство по технологическому развитию</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596078</t>
+          <t xml:space="preserve">    598230</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>"Максимальное количество пользователей модуля "Интеграция с ПОС", разрешенное лицензиией, превышено на 70", при публикации решения МЭДО</t>
+          <t>"Запись с идентификатором 0 не найдена" при открытий карточки входящего письма.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Переадресовано</t>
+          <t>На контроле</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Пестрикова Валерия</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>9.82</v>
+        <v>4.83</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -39490,19 +39671,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Агентство по технологическому развитию</t>
+          <t>АрмаДок ООО</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595891</t>
+          <t xml:space="preserve">    599224</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>"Трназакция откатилась", при отправке Вх письма на согласование</t>
+          <t>"Object does not match target type." при согласовании договора. ИД ошибки e0839226-ed1144.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -39512,32 +39693,32 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>8.58</v>
+        <v>4.17</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Низкий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Гарант-Чебоксары</t>
+          <t>Подводные Технологии и Ремонт - Центр Передового Опыта ООО</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596279</t>
+          <t xml:space="preserve">    599509</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>При выгрузке документов с открепленной ЭП расходится время подписания и установки штампа времени</t>
+          <t>Не запускается программа у всех пользователей. Сервер перезагружали. Ошибка IS-Builder Runtime Environment не отвечает</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -39551,42 +39732,43 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8.029999999999999</v>
+        <v>3.37</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Низкий</t>
+          <t>Высокий</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>СТАРКОВ Групп ООО</t>
+          <t>Администрация г. Киров</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596434</t>
+          <t xml:space="preserve">    599327</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>В решении «База знаний» в области знаний отображается некорректное время редактирование статей +4 часа от Ижевского времени</t>
+          <t xml:space="preserve">
+Входящие пакеты по МЭДО не переносятся их очереди In в Loaded</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>В работе</t>
+          <t>На контроле</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Пестрикова Валерия</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>3.15</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -39595,19 +39777,19 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>РосА Ижевск</t>
+          <t>Агентство по технологическому развитию</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596285</t>
+          <t xml:space="preserve">    597977</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Служба ввода прекращает работу, при нехватке прав  на документ в папке захвата</t>
+          <t>При обработке пакетов МЭДО возникает ошибка: Ошибка при обработке пакетов МЭДО: Object reference not set to an instance of an object.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -39617,11 +39799,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Пестрикова Валерия</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>6.73</v>
+        <v>2.93</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -39630,33 +39812,33 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Гарант-Чебоксары</t>
+          <t>Государственное учреждение информационных технологий и телекоммуникаций Омской области (ГУИТ КУ)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596424</t>
+          <t xml:space="preserve">    599679</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Не запускаются сервисные службы Directum 5.8.8, после установки</t>
+          <t>Сотрудник аннулировал документ в ЭДО, ему пришло задание на обработку. Задание выполнили, но статус "Аннулирован" в документе не проставился + не пришло задание на доработку (висит на контроле возврата).</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>В работе</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Банников Константин</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>6.47</v>
+        <v>2.45</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -39665,24 +39847,24 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Миррико менеджмент ООО (Mirrico)</t>
+          <t>Гарант-Чебоксары</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596483</t>
+          <t xml:space="preserve">    599303</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>"Eroare a prelucrarii comenzii serviciului depozitelor de fisiere pe "SBE164.maib.local"" при первом открытии документа в Directum</t>
+          <t>[DTC#098790][EXT#2686] Ошибка Ario "Object reference not set to an instance of an object" при попытке обработать обращения с электронной почты</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>Переадресовано</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -39691,7 +39873,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6.12</v>
+        <v>2.28</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -39700,19 +39882,19 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Молдова Агроиндбанк (Moldova Agroindbank)</t>
+          <t>Центр цифровых технологий УР (АУ ЦЦТ УР) (ПУР) (бывш. АУ РИЦ УР)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596413</t>
+          <t xml:space="preserve">    599321</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Не открывается задание на доработку у инициатора</t>
+          <t>Не создаются задания. Система развернута с нуля на AstraLinux по инструкции администратора Linux. Сервисы, mongo и rabbit функционируют.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -39722,32 +39904,32 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Пестрикова Валерия</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>5.93</v>
+        <v>1.93</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Средний</t>
+          <t>Низкий</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Акелон ООО (Akelon)</t>
+          <t>Находка-АИС ООО</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596486</t>
+          <t xml:space="preserve">    598751</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Сотрудник который согласовал документ по задаче не подтянулся в лист согласования</t>
+          <t xml:space="preserve"> Не могу войти в программу, не входил уже более 3 месяцев</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -39757,32 +39939,32 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Зверев Иван</t>
+          <t>Русских Руслан</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>5.43</v>
+        <v>1.25</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Низкий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Гарант-Чебоксары</t>
+          <t>Владимирская Областная Станция По Борьбе С Болезнями Животных (СББЖ) ГБУ</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">    589701</t>
+          <t xml:space="preserve">    599641</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Прекращение задач, которые ранее поступили на пользователя Станчина Т.О. на приемку резолюции.</t>
+          <t>При поступлении входящих документов по МЭДО происходит сопоставление, регистрация и подбор журнала исходящих писем.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -39792,11 +39974,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Пестрикова Валерия</t>
+          <t>Банников Константин</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>4.95</v>
+        <v>1.05</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -39805,19 +39987,19 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Министерство промышленности и научно-технического развития Омской области (Минпром Омской области)</t>
+          <t>Администрация Губернатора Владимирской области</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595629</t>
+          <t xml:space="preserve">    599583</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Не отправляются из РК исходящие документы контрагентам</t>
+          <t>System.ServiceModel.ServiceActivationException: Не удается активировать запрошенную службу "http://localhost/Sungero/CommonService.svc/pw при запуске DrxUtil</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -39827,336 +40009,20 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>4.68</v>
+        <v>0.17</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Низкий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>СТАРКОВ Групп ООО</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596428</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>"Внутренняя ошибка сервера ", при нажатии на кнопку перекомплектовать</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>3.95</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Гарант-Чебоксары</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596388</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>В описании нового функционала системы опечатки</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Министерство промышленности и научно-технического развития Омской области (Минпром Омской области)</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    595765</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Ошибка "Object reference not set to an instance of an object" при синхронизация контрагентов</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>2.85</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Гарант-Чебоксары</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596524</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Некорректное отображение спецсимволов после преобразования в pdf</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>В работе</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>1.98</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Гарант-Чебоксары</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596129</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Продолжение обращения №595226.
- "Веб-сервис недоступен или указан неверный адрес", при попытке подключиться к серверу sedo.omskportal.ru/nomad с мобильного приложения Directum Solo</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Министерство промышленности и научно-технического развития Омской области (Минпром Омской области)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596545</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Замечание к справке системы Directum RX версии 4.6</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>В работе</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Банников Константин</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>АрмаДок ООО</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596559</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>"The controller for path '…' was not found or does not implement IControlle" в логах сервера Nomad</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Бобылев Сергей</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Низкий</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Интант ООО</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596044</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Не работает функция заполнения карточки контрагента через кнопку "Заполнить по ИНН/ОГРН".</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Банников Константин</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Средний</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Локато Док ООО</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    596420</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Некорректное отображение наименования в листе согласования</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>На контроле</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Банников Константин</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Низкий</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>АрмаДок ООО</t>
+          <t>ЕАЕ-Консалт (EAE Consulting)</t>
         </is>
       </c>
     </row>
@@ -40171,7 +40037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40228,12 +40094,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595879</t>
+          <t xml:space="preserve">    598804</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Периодически выкидывает пользователей из системы после отключения ClientsConnectionService и SungeroCentrifugo</t>
+          <t>Консультация по настройке внешней аутентификации на выделенном облачном стенде</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -40247,7 +40113,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>30.28</v>
+        <v>19.43</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -40256,19 +40122,19 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ДиБиЭй ООО (DBA)</t>
+          <t>ЦИТ Проекты и Решения</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595305</t>
+          <t xml:space="preserve">    598084</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Как можно отследить активности пользователей системы Directum?</t>
+          <t>В каком формате должна передаваться МЧД при обмене через МЭДО ? Передаваться просто как приложение ?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -40278,11 +40144,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Пестрикова Валерия</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>20.62</v>
+        <v>15.68</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -40291,33 +40157,33 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ВДГБ-Аудит</t>
+          <t>ТАНАИС ООО</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595535</t>
+          <t xml:space="preserve">    599247</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Каким инструментом мониторинга системы или уведомлений можно воспользоваться для выявления ошибок отправки писем сценария</t>
+          <t>Скрипт, указанный в справке, дает нулевой запрос при username-аутентификации.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>В работе</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Зверев Иван</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>14.52</v>
+        <v>15.3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -40326,19 +40192,19 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Центр внедрения документооборота (ЦВД)</t>
+          <t>Новаком Системс</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596036</t>
+          <t xml:space="preserve">    598850</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>"Ошибка NETSDK1045 текущий пакет SDK для .NET не поддерживает целевой объект .NET 6.0", при сборке RXCmd</t>
+          <t>Консультация по вопросу перехода на МЧД.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -40348,11 +40214,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Зверев Иван</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>13.48</v>
+        <v>14.85</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -40361,33 +40227,34 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ЕАЕ-Консалт (EAE Consulting)</t>
+          <t>ТАНАИС ООО</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595521</t>
+          <t xml:space="preserve">    598055</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>При попытке открыть страницу сервера приложений http://server/sp/CommonService.svc получаем 503 ошибку.</t>
+          <t>Продолжение обращения №597445.
+  Не доступен Региональный портал госуслуг (https://pgu.omskportal.ru/) при включенном кэшировании.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>Переадресовано</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Пестрикова Валерия</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
+        <v>14.15</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -40396,19 +40263,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ЦИТ Проекты и Решения</t>
+          <t>Министерство промышленности и научно-технического развития Омской области (Минпром Омской области)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595005</t>
+          <t xml:space="preserve">    599348</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Зависает система Directum через сутки после перезапуска сервера</t>
+          <t>Взаимная блокировка асинхроников выдачи прав с разных плеч кластера</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -40418,46 +40285,46 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>11.72</v>
+        <v>12.5</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Высокий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Министерство цифрового развития, информационных технологий и связи Рязанской области</t>
+          <t>СТАРКОВ Групп ООО</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595434</t>
+          <t xml:space="preserve">    599500</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Реализована ли возможность обмена с клиентами ГИС «ТОР СЭД» в коннекторе МЭДО ?</t>
+          <t>Каким образом в аналитическом многостраничном отчете в форме таблицы, разработанном в Fastreport для RX, исключить автоматически добавляемый разрыв страницы и соответственно разрыв таблицы.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>В работе</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>11.48</v>
+        <v>12.38</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -40466,33 +40333,33 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ТАНАИС ООО</t>
+          <t>Новаком Системс</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    592801</t>
+          <t xml:space="preserve">    599543</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Продолжение обращения №583834."При загрузке квитанции не удалось найти пакет или уведомление", в работе МЭДО</t>
+          <t>По истечении работы веб-доступа порядка 12 часов начинаются ошибки и блокировки процессов, после чего войти в веб-доступ невозможно. ошибка Не удалось получить фабрику класса COM для компонента с CLSID {0A790054-8E2E-4099-8B1F-2F0492F97194}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>На контроле</t>
+          <t>В работе</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Пестрикова Валерия</t>
+          <t>Бобылев Сергей</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>10.95</v>
+        <v>11.83</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -40501,19 +40368,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>АрмаДок ООО</t>
+          <t>Интеллектика</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596077</t>
+          <t xml:space="preserve">    597192</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Поддерживает ли директум возможность дешифрования зашифрованных документов?</t>
+          <t>Ошибка Microsoft.WebTools.Shared.Exceptions.WebToolsException при публикации RxCmdPluginSDK.zip в Visual Studio 2019</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -40527,7 +40394,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>10.88</v>
+        <v>11.75</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -40536,19 +40403,19 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>ДЖИДИЭС ООО (JDSolutions Джиди Решения)</t>
+          <t>ЕАЕ-Консалт (EAE Consulting)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595714</t>
+          <t xml:space="preserve">    599569</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ошибка "Без действующей лицензии с системой может работать ограниченное количество пользователей" при вынесении сервиса nomad на отдельный сервер.</t>
+          <t>Консультация по необходимости перемещения документов при предупреждении "Изменился адрес сервиса хранилищ. Документы из старого хранилища должны быть перемещены вручную..." после изменения адреса сервиса хранилищ</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -40558,32 +40425,32 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Банников Константин</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7.77</v>
+        <v>8.83</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Низкий</t>
+          <t>Планируемый</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ДиБиЭй ООО (DBA)</t>
+          <t>Удостоверяющий центр ГАЗИНФОРМСЕРВИС (УЦ ГИС)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595723</t>
+          <t xml:space="preserve">    598083</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Что необходимо сделать, чтобы при отправке, документ  отправлялся с помощью оператора ЭДО "ЭДИСОФТ".</t>
+          <t>Смогут ли граждане при получении ответа на свое обращение, произвести проверку КЭП документа, на портале гос. Услуг без МЧД?</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -40597,7 +40464,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>6.43</v>
+        <v>6.03</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -40606,19 +40473,19 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Гарант-Чебоксары</t>
+          <t>ТАНАИС ООО</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    596276</t>
+          <t xml:space="preserve">    598079</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Если в разработке свойство из коллекции сделать обязательным, затем изменить обратно на необязательное, состояние не меняется и система требует его заполнения</t>
+          <t>Для каких видов документов обязательно использование МЧД?</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -40632,7 +40499,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>5.97</v>
+        <v>6.02</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -40641,19 +40508,19 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>СТАРКОВ Групп ООО</t>
+          <t>ТАНАИС ООО</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595550</t>
+          <t xml:space="preserve">    599262</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Не поступает широковещательная рассылка по ВС ФНС</t>
+          <t>Warning! Do not use this Postgres container for production environment! For test env only при установке системы</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -40663,33 +40530,32 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Бобылев Сергей</t>
+          <t>Зверев Иван</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4.82</v>
+        <v>5.08</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Высокий</t>
+          <t>Средний</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Государственное учреждение информационных технологий и телекоммуникаций Омской области (ГУИТ КУ)</t>
+          <t>Новаком Системс</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    595006</t>
+          <t xml:space="preserve">    599052</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Необходимо удалить все задачи, задания, а так же запросы по 31.12.2020 включительно.</t>
+          <t>Как очистить БД Directum от данных?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -40703,7 +40569,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3.87</v>
+        <v>5.07</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -40712,7 +40578,147 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Министерство цифрового развития, информационных технологий и связи Рязанской области</t>
+          <t>Востсибнефтегаз АО (Восточно-Сибирская нефтегазовая компания (ВСНК) (РН РиД)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    597914</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>На agile-доске тикеты пустые</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>На контроле</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Пестрикова Валерия</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>ЦИТ Проекты и Решения</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    599605</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>"Cannot load the certificate's '46D6AF8273302D40B1E1A48ED61A685E1EA662E8' private key from file" при попытке подписать на MacOS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>На контроле</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Бобылев Сергей</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>ЦИТ Проекты и Решения</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    599433</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Настроен фоновый процесс "Документооборот. Рассылка писем о новых и просроченных заданиях" с параметрами запуска раз в 30 минут. Но уведомления о просроченном задании приходит только 1 раз.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>На контроле</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Бобылев Сергей</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ЦИТ Проекты и Решения</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    599423</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ошибка при публикации решения после удаления перекрытия</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>На контроле</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Зверев Иван</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Средний</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Костромская сбытовая компания ПАО</t>
         </is>
       </c>
     </row>
@@ -40727,7 +40733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40769,57 +40775,109 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>24.03.2023</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    589701</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Прекращение задач, которые ранее поступили на пользователя Станчина Т.О. на приемку резолюции.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>На контроле</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" style="1" min="1" max="1"/>
+    <col width="20" customWidth="1" style="1" min="2" max="2"/>
+    <col width="100" customWidth="1" style="1" min="3" max="3"/>
+    <col width="25" customWidth="1" style="1" min="4" max="4"/>
+    <col width="25" customWidth="1" style="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Дата поступления</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Номер</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Описание</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ответственный</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Состояние</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>21.04.2023</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    592801</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Продолжение обращения №583834."При загрузке квитанции не удалось найти пакет или уведомление", в работе МЭДО</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Пестрикова Валерия</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>На контроле</t>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" style="1" min="1" max="1"/>
+    <col width="20" customWidth="1" style="1" min="2" max="2"/>
+    <col width="100" customWidth="1" style="1" min="3" max="3"/>
+    <col width="25" customWidth="1" style="1" min="4" max="4"/>
+    <col width="25" customWidth="1" style="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Дата поступления</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Номер</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Описание</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Ответственный</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Состояние</t>
         </is>
       </c>
     </row>

</xml_diff>